<commit_message>
changes for displaying structure
</commit_message>
<xml_diff>
--- a/SwitchportList.xlsx
+++ b/SwitchportList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateu\Desktop\PROGRAMOWANIE\Praktyki\Kamery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B209CCA9-2CE7-4CE8-ADF2-C42F4437449E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6825F2A1-452B-4E80-9F58-6BA4EF97F0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1CCA29BD-11D6-4AD7-A7FB-25F66BEEDD13}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>S1/10.1.10</t>
   </si>
@@ -80,15 +80,6 @@
     <t>opis</t>
   </si>
   <si>
-    <t>kontenery</t>
-  </si>
-  <si>
-    <t>stolarnia</t>
-  </si>
-  <si>
-    <t>plac stolarnia</t>
-  </si>
-  <si>
     <t>stoly jumbo front</t>
   </si>
   <si>
@@ -137,12 +128,6 @@
     <t>10.1.30.21 p18</t>
   </si>
   <si>
-    <t>kontenery II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stolarnia II </t>
-  </si>
-  <si>
     <t>plac stolarnia II</t>
   </si>
   <si>
@@ -168,6 +153,18 @@
   </si>
   <si>
     <t>10.1.30.21 p24</t>
+  </si>
+  <si>
+    <t>kontenery produkcyjne firmy</t>
+  </si>
+  <si>
+    <t>czesc stolarniana firmy</t>
+  </si>
+  <si>
+    <t>plac poza stolarnia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hala cnc duzy maszyna </t>
   </si>
 </sst>
 </file>
@@ -543,7 +540,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +577,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -594,7 +591,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -608,7 +605,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -622,7 +619,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -636,7 +633,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -650,7 +647,7 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -664,7 +661,7 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -678,7 +675,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -692,7 +689,7 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -706,7 +703,7 @@
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -717,10 +714,10 @@
         <v>158</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -731,10 +728,10 @@
         <v>157</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -745,10 +742,10 @@
         <v>156</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -759,10 +756,10 @@
         <v>155</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -773,10 +770,10 @@
         <v>154</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -787,10 +784,10 @@
         <v>153</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -801,10 +798,10 @@
         <v>152</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -815,10 +812,10 @@
         <v>151</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -829,10 +826,10 @@
         <v>150</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -843,10 +840,10 @@
         <v>149</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>